<commit_message>
Added excel writing script
</commit_message>
<xml_diff>
--- a/TestDataUtility/TestData.xlsx
+++ b/TestDataUtility/TestData.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prem\eclipse-workspace\TutorialNinjaAutomation\TestDataUtility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D1EBC3-FD96-46C0-8875-7A77A5CD8F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E628F262-19A4-4A75-B303-404E33F143C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="3000" windowWidth="18900" windowHeight="10965" xr2:uid="{3258FADF-DB88-40D8-858F-18CDAF9F31C3}"/>
+    <workbookView xWindow="2910" yWindow="3615" windowWidth="18900" windowHeight="10965" xr2:uid="{3258FADF-DB88-40D8-858F-18CDAF9F31C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -49,12 +49,19 @@
   </si>
   <si>
     <t>shameer@gmail.com</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,7 +87,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +98,32 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -122,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,6 +166,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -448,20 +489,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7F7BC4F-FF6D-4425-95C9-9EE0FFBB74D9}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.85546875"/>
+    <col min="2" max="2" customWidth="true" width="17.28515625"/>
+    <col min="3" max="3" customWidth="true" width="12.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +512,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -482,8 +524,11 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s" s="9">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -493,8 +538,11 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" t="s" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -503,6 +551,9 @@
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" t="s" s="11">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Extent report conifiguration
</commit_message>
<xml_diff>
--- a/TestDataUtility/TestData.xlsx
+++ b/TestDataUtility/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prem\eclipse-workspace\TutorialNinjaAutomation\TestDataUtility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E628F262-19A4-4A75-B303-404E33F143C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C141E36B-A00E-4640-B815-5AF230441906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2910" yWindow="3615" windowWidth="18900" windowHeight="10965" xr2:uid="{3258FADF-DB88-40D8-858F-18CDAF9F31C3}"/>
   </bookViews>
@@ -155,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,7 +166,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
@@ -492,7 +491,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +523,7 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="9">
+      <c r="D2" t="s" s="8">
         <v>8</v>
       </c>
     </row>
@@ -538,7 +537,7 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s" s="10">
+      <c r="D3" t="s" s="9">
         <v>9</v>
       </c>
     </row>
@@ -552,7 +551,7 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" t="s" s="10">
         <v>9</v>
       </c>
     </row>

</xml_diff>